<commit_message>
Commint before final simulations
</commit_message>
<xml_diff>
--- a/results/Optimal L for Charts.xlsx
+++ b/results/Optimal L for Charts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\uh09200086.bmwgroup.net\home$\QXZ3G2L\Masters\Main_Code\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QXZ3G2L\Documents\Masters\Main_Code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E6B2F9-96B3-4ECA-AA5A-91C316C58E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0ABF6A-C1A7-4C02-B1B1-E7B073ACF442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Univariate Charts" sheetId="1" r:id="rId1"/>
@@ -64,6 +64,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,12 +389,12 @@
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -422,7 +426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -496,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2.5139999999999998</v>
       </c>
@@ -519,6 +523,15 @@
         <v>0.01</v>
       </c>
       <c r="I3" s="1"/>
+      <c r="K3" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
       <c r="P3" s="1">
         <v>2.4830000000000001</v>
       </c>
@@ -543,8 +556,17 @@
       <c r="X3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z3" s="2">
+        <v>2.8015625000000002</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2.7669999999999999</v>
       </c>
@@ -567,6 +589,15 @@
         <v>0.05</v>
       </c>
       <c r="I4" s="1"/>
+      <c r="K4" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
       <c r="P4" s="1">
         <v>2.6869999999999998</v>
       </c>
@@ -591,8 +622,17 @@
       <c r="X4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z4" s="2">
+        <v>2.8080078099999999</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2.8069999999999999</v>
       </c>
@@ -615,6 +655,15 @@
         <v>0.09</v>
       </c>
       <c r="I5" s="1"/>
+      <c r="K5" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
       <c r="P5" s="1">
         <v>2.778</v>
       </c>
@@ -639,8 +688,17 @@
       <c r="X5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z5" s="2">
+        <v>2.8015625000000002</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AC5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F6" s="1">
         <v>2.7719999999999998</v>
       </c>
@@ -651,6 +709,15 @@
         <v>0.05</v>
       </c>
       <c r="I6" s="1"/>
+      <c r="K6" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
       <c r="U6" s="1">
         <v>2.2530000000000001</v>
       </c>
@@ -663,8 +730,17 @@
       <c r="X6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z6" s="2">
+        <v>2.8015625000000002</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F7" s="1">
         <v>2.7629999999999999</v>
       </c>
@@ -675,6 +751,15 @@
         <v>0.1</v>
       </c>
       <c r="I7" s="1"/>
+      <c r="K7" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
       <c r="U7" s="1">
         <v>2.395</v>
       </c>
@@ -687,8 +772,17 @@
       <c r="X7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z7" s="2">
+        <v>2.8058593799999998</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AC7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F8" s="1">
         <v>2.762</v>
       </c>
@@ -699,6 +793,15 @@
         <v>0.2</v>
       </c>
       <c r="I8" s="1"/>
+      <c r="K8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
       <c r="U8" s="1">
         <v>2.5270000000000001</v>
       </c>
@@ -711,8 +814,17 @@
       <c r="X8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z8" s="2">
+        <v>2.8058593799999998</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AC8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F9" s="1">
         <v>2.8039999999999998</v>
       </c>
@@ -723,6 +835,15 @@
         <v>0.05</v>
       </c>
       <c r="I9" s="1"/>
+      <c r="K9" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
       <c r="U9" s="1">
         <v>2.7050000000000001</v>
       </c>
@@ -735,8 +856,17 @@
       <c r="X9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z9" s="2">
+        <v>2.8015625000000002</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F10" s="1">
         <v>2.8029999999999999</v>
       </c>
@@ -747,6 +877,15 @@
         <v>0.1</v>
       </c>
       <c r="I10" s="1"/>
+      <c r="K10" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
       <c r="U10" s="1">
         <v>2.6509999999999998</v>
       </c>
@@ -759,8 +898,17 @@
       <c r="X10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z10" s="2">
+        <v>2.8058593799999998</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AC10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F11" s="1">
         <v>2.794</v>
       </c>
@@ -771,6 +919,15 @@
         <v>0.25</v>
       </c>
       <c r="I11" s="1"/>
+      <c r="K11" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
       <c r="U11" s="1">
         <v>2.625</v>
       </c>
@@ -783,8 +940,17 @@
       <c r="X11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z11" s="2">
+        <v>2.8058593799999998</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AC11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F12" s="1">
         <v>2.8039999999999998</v>
       </c>
@@ -795,8 +961,26 @@
         <v>0.05</v>
       </c>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>2.7994140600000001</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F13" s="1">
         <v>2.8090000000000002</v>
       </c>
@@ -807,8 +991,26 @@
         <v>0.1</v>
       </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="K13" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>2.79296875</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AC13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="F14" s="1">
         <v>2.8010000000000002</v>
       </c>
@@ -819,6 +1021,24 @@
         <v>0.25</v>
       </c>
       <c r="I14" s="1"/>
+      <c r="K14" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>2.8015625000000002</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AC14">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed L values to be saved in json files
</commit_message>
<xml_diff>
--- a/results/Optimal L for Charts.xlsx
+++ b/results/Optimal L for Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QXZ3G2L\Documents\Masters\Main_Code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0ABF6A-C1A7-4C02-B1B1-E7B073ACF442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAC0AFE-6A1E-463B-BB8D-762577B67BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Univariate Charts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="11">
   <si>
     <t>Phi</t>
   </si>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -105,7 +105,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,13 +388,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -426,7 +426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -500,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2.5139999999999998</v>
       </c>
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="U3" s="1">
-        <v>2.399</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="V3" s="1">
         <v>0.1</v>
@@ -566,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2.7669999999999999</v>
       </c>
@@ -611,7 +611,7 @@
         <v>9</v>
       </c>
       <c r="U4" s="1">
-        <v>2.105</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="V4" s="1">
         <v>0.1</v>
@@ -632,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2.8069999999999999</v>
       </c>
@@ -677,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="U5" s="1">
-        <v>2.31</v>
+        <v>2.54</v>
       </c>
       <c r="V5" s="1">
         <v>0.1</v>
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F6" s="1">
         <v>2.7719999999999998</v>
       </c>
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="U6" s="1">
-        <v>2.2530000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="V6" s="1">
         <v>0.25</v>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F7" s="1">
         <v>2.7629999999999999</v>
       </c>
@@ -761,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="U7" s="1">
-        <v>2.395</v>
+        <v>2.72</v>
       </c>
       <c r="V7" s="1">
         <v>0.25</v>
@@ -782,7 +782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F8" s="1">
         <v>2.762</v>
       </c>
@@ -803,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="U8" s="1">
-        <v>2.5270000000000001</v>
+        <v>2.73</v>
       </c>
       <c r="V8" s="1">
         <v>0.25</v>
@@ -824,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F9" s="1">
         <v>2.8039999999999998</v>
       </c>
@@ -845,13 +845,13 @@
         <v>1</v>
       </c>
       <c r="U9" s="1">
-        <v>2.7050000000000001</v>
+        <v>2.78</v>
       </c>
       <c r="V9" s="1">
         <v>0.5</v>
       </c>
       <c r="W9" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>9</v>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F10" s="1">
         <v>2.8029999999999999</v>
       </c>
@@ -887,13 +887,13 @@
         <v>2</v>
       </c>
       <c r="U10" s="1">
-        <v>2.6509999999999998</v>
+        <v>2.78</v>
       </c>
       <c r="V10" s="1">
         <v>0.5</v>
       </c>
       <c r="W10" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="X10" s="1" t="s">
         <v>9</v>
@@ -908,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F11" s="1">
         <v>2.794</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0.5</v>
       </c>
       <c r="W11" s="1">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="X11" s="1" t="s">
         <v>9</v>
@@ -950,7 +950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
         <v>2.8039999999999998</v>
       </c>
@@ -970,6 +970,18 @@
       <c r="N12">
         <v>1</v>
       </c>
+      <c r="U12" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="Z12" s="2">
         <v>2.7994140600000001</v>
       </c>
@@ -980,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F13" s="1">
         <v>2.8090000000000002</v>
       </c>
@@ -1000,6 +1012,18 @@
       <c r="N13">
         <v>2</v>
       </c>
+      <c r="U13" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="Z13" s="2">
         <v>2.79296875</v>
       </c>
@@ -1010,7 +1034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F14" s="1">
         <v>2.8010000000000002</v>
       </c>
@@ -1029,6 +1053,18 @@
       </c>
       <c r="N14">
         <v>4</v>
+      </c>
+      <c r="U14" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="Z14" s="2">
         <v>2.8015625000000002</v>

</xml_diff>